<commit_message>
Cambios en Posición diaria de bancos para totalizadores por mes.
</commit_message>
<xml_diff>
--- a/Conciliacion/App_Web/Sitio Conicliacion 07-07-2017/SitioConciliacion/InformesExcel/PosicionDiariaGOA012018.xlsx
+++ b/Conciliacion/App_Web/Sitio Conicliacion 07-07-2017/SitioConciliacion/InformesExcel/PosicionDiariaGOA012018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Reporte
 POSICION DIARIA DE BANCOS</t>
@@ -33,7 +33,7 @@
     <t>LUNES</t>
   </si>
   <si>
-    <t>CAJA CAJA HUATULCO</t>
+    <t>CAJA HUATULCO</t>
   </si>
   <si>
     <t>KILOS</t>
@@ -159,13 +159,19 @@
     <t>TARJETA BANORTE 0671084374</t>
   </si>
   <si>
-    <t>CAJA CAJA 7</t>
-  </si>
-  <si>
-    <t>CAJA TESORERIA</t>
-  </si>
-  <si>
-    <t>CAJA TOTAL</t>
+    <t>CAJA 7</t>
+  </si>
+  <si>
+    <t>TESORERIA</t>
+  </si>
+  <si>
+    <t>TOTAL MES</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>junio</t>
   </si>
 </sst>
 </file>
@@ -373,17 +379,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5318363734654" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5318363734654" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5318363734654" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.5318363734654" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -581,63 +584,63 @@
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="6" t="e">
-        <f>=SUM(C4:C14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" s="6" t="e">
-        <f>=SUM(E4:E14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" s="6" t="e">
-        <f>=SUM(G4:G14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" s="6" t="e">
-        <f>=SUM(I4:I14)</f>
-        <v>#VALUE!</v>
+      <c r="C16" s="6">
+        <f>SUM(C4:C14)</f>
+        <v>229291</v>
+      </c>
+      <c r="E16" s="6">
+        <f>SUM(E4:E14)</f>
+        <v>194144.99</v>
+      </c>
+      <c r="G16" s="6">
+        <f>SUM(G4:G14)</f>
+        <v>37727.55</v>
+      </c>
+      <c r="I16" s="6">
+        <f>SUM(I4:I14)</f>
+        <v>298251.12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="6" t="e">
-        <f>=SUM(C8:C11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" s="6" t="e">
-        <f>=SUM(E8:E11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" s="6" t="e">
-        <f>=SUM(G8:G11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I17" s="6" t="e">
-        <f>=SUM(I8:I11)</f>
-        <v>#VALUE!</v>
+      <c r="C17" s="6">
+        <f>SUM(C8:C11)</f>
+        <v>41429.48</v>
+      </c>
+      <c r="E17" s="6">
+        <f>SUM(E8:E11)</f>
+        <v>46651.13</v>
+      </c>
+      <c r="G17" s="6">
+        <f>SUM(G8:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <f>SUM(I8:I11)</f>
+        <v>75914.59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="6" t="e">
-        <f>=SUM(C16:C16)-SUM(C17:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="6" t="e">
-        <f>=SUM(E16:E16)-SUM(E17:E17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="6" t="e">
-        <f>=SUM(G16:G16)-SUM(G17:G17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="6" t="e">
-        <f>=SUM(I16:I16)-SUM(I17:I17)</f>
-        <v>#VALUE!</v>
+      <c r="C19" s="6">
+        <f>SUM(C16:C16)-SUM(C17:C17)</f>
+        <v>187861.52</v>
+      </c>
+      <c r="E19" s="6">
+        <f>SUM(E16:E16)-SUM(E17:E17)</f>
+        <v>147493.86</v>
+      </c>
+      <c r="G19" s="6">
+        <f>SUM(G16:G16)-SUM(G17:G17)</f>
+        <v>37727.55</v>
+      </c>
+      <c r="I19" s="6">
+        <f>SUM(I16:I16)-SUM(I17:I17)</f>
+        <v>222336.53</v>
       </c>
     </row>
     <row r="21">
@@ -682,7 +685,7 @@
         <v>165261.9</v>
       </c>
       <c r="I23" s="6">
-        <v>59419.12</v>
+        <v>63582.62</v>
       </c>
     </row>
     <row r="24">
@@ -728,84 +731,84 @@
       <c r="A30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="6" t="e">
-        <f>=SUM(C21:C29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" s="6" t="e">
-        <f>=SUM(E21:E29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" s="6" t="e">
-        <f>=SUM(G21:G29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="6" t="e">
-        <f>=SUM(I21:I29)</f>
-        <v>#VALUE!</v>
+      <c r="C30" s="6">
+        <f>SUM(C21:C29)</f>
+        <v>1489764.74</v>
+      </c>
+      <c r="E30" s="6">
+        <f>SUM(E21:E29)</f>
+        <v>869844.91</v>
+      </c>
+      <c r="G30" s="6">
+        <f>SUM(G21:G29)</f>
+        <v>85229.55</v>
+      </c>
+      <c r="I30" s="6">
+        <f>SUM(I21:I29)</f>
+        <v>1685977.11</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="6" t="e">
-        <f>=SUM(C25:C27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="6" t="e">
-        <f>=SUM(E25:E27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" s="6" t="e">
-        <f>=SUM(G25:G27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="6" t="e">
-        <f>=SUM(I25:I27)</f>
-        <v>#VALUE!</v>
+      <c r="C31" s="6">
+        <f>SUM(C25:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <f>SUM(E25:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
+        <f>SUM(G25:G27)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="6">
+        <f>SUM(I25:I27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="6" t="e">
-        <f>=SUM(C30:C30)-SUM(C31:C31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E32" s="6" t="e">
-        <f>=SUM(E30:E30)-SUM(E31:E31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G32" s="6" t="e">
-        <f>=SUM(G30:G30)-SUM(G31:G31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I32" s="6" t="e">
-        <f>=SUM(I30:I30)-SUM(I31:I31)</f>
-        <v>#VALUE!</v>
+      <c r="C32" s="6">
+        <f>SUM(C30:C30)-SUM(C31:C31)</f>
+        <v>1489764.74</v>
+      </c>
+      <c r="E32" s="6">
+        <f>SUM(E30:E30)-SUM(E31:E31)</f>
+        <v>869844.91</v>
+      </c>
+      <c r="G32" s="6">
+        <f>SUM(G30:G30)-SUM(G31:G31)</f>
+        <v>85229.55</v>
+      </c>
+      <c r="I32" s="6">
+        <f>SUM(I30:I30)-SUM(I31:I31)</f>
+        <v>1685977.11</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="6" t="e">
-        <f>=SUM(C19:C19)-SUM(C32:C32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" s="6" t="e">
-        <f>=SUM(E19:E19)-SUM(E32:E32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" s="6" t="e">
-        <f>=SUM(G19:G19)-SUM(G32:G32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I34" s="6" t="e">
-        <f>=SUM(I19:I19)-SUM(I32:I32)</f>
-        <v>#VALUE!</v>
+      <c r="C34" s="6">
+        <f>SUM(C19:C19)-SUM(C32:C32)</f>
+        <v>-1301903.22</v>
+      </c>
+      <c r="E34" s="6">
+        <f>SUM(E19:E19)-SUM(E32:E32)</f>
+        <v>-722351.05</v>
+      </c>
+      <c r="G34" s="6">
+        <f>SUM(G19:G19)-SUM(G32:G32)</f>
+        <v>-47502</v>
+      </c>
+      <c r="I34" s="6">
+        <f>SUM(I19:I19)-SUM(I32:I32)</f>
+        <v>-1463640.58</v>
       </c>
     </row>
     <row r="35">
@@ -926,13 +929,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5318363734654" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5318363734654" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5318363734654" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="11.5318363734654" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1137,63 +1140,63 @@
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="21" t="e">
-        <f>=SUM(C4:C14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" s="21" t="e">
-        <f>=SUM(E4:E14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" s="21" t="e">
-        <f>=SUM(G4:G14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" s="21" t="e">
-        <f>=SUM(I4:I14)</f>
-        <v>#VALUE!</v>
+      <c r="C16" s="21">
+        <f>SUM(C4:C14)</f>
+        <v>255180.85</v>
+      </c>
+      <c r="E16" s="21">
+        <f>SUM(E4:E14)</f>
+        <v>300458.75999999995</v>
+      </c>
+      <c r="G16" s="21">
+        <f>SUM(G4:G14)</f>
+        <v>72745.2</v>
+      </c>
+      <c r="I16" s="21">
+        <f>SUM(I4:I14)</f>
+        <v>311393.22</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="21" t="e">
-        <f>=SUM(C8:C11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" s="21" t="e">
-        <f>=SUM(E8:E11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" s="21" t="e">
-        <f>=SUM(G8:G11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I17" s="21" t="e">
-        <f>=SUM(I8:I11)</f>
-        <v>#VALUE!</v>
+      <c r="C17" s="21">
+        <f>SUM(C8:C11)</f>
+        <v>24179.66</v>
+      </c>
+      <c r="E17" s="21">
+        <f>SUM(E8:E11)</f>
+        <v>36264.36</v>
+      </c>
+      <c r="G17" s="21">
+        <f>SUM(G8:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="21">
+        <f>SUM(I8:I11)</f>
+        <v>21756.63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="21" t="e">
-        <f>=SUM(C16:C16)-SUM(C17:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="21" t="e">
-        <f>=SUM(E16:E16)-SUM(E17:E17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="21" t="e">
-        <f>=SUM(G16:G16)-SUM(G17:G17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I19" s="21" t="e">
-        <f>=SUM(I16:I16)-SUM(I17:I17)</f>
-        <v>#VALUE!</v>
+      <c r="C19" s="21">
+        <f>SUM(C16:C16)-SUM(C17:C17)</f>
+        <v>231001.19</v>
+      </c>
+      <c r="E19" s="21">
+        <f>SUM(E16:E16)-SUM(E17:E17)</f>
+        <v>264194.39999999997</v>
+      </c>
+      <c r="G19" s="21">
+        <f>SUM(G16:G16)-SUM(G17:G17)</f>
+        <v>72745.2</v>
+      </c>
+      <c r="I19" s="21">
+        <f>SUM(I16:I16)-SUM(I17:I17)</f>
+        <v>289636.58999999997</v>
       </c>
     </row>
     <row r="21">
@@ -1281,84 +1284,84 @@
       <c r="A30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="21" t="e">
-        <f>=SUM(C21:C29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" s="21" t="e">
-        <f>=SUM(E21:E29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" s="21" t="e">
-        <f>=SUM(G21:G29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="21" t="e">
-        <f>=SUM(I21:I29)</f>
-        <v>#VALUE!</v>
+      <c r="C30" s="21">
+        <f>SUM(C21:C29)</f>
+        <v>2000272.3699999999</v>
+      </c>
+      <c r="E30" s="21">
+        <f>SUM(E21:E29)</f>
+        <v>1106303.8900000001</v>
+      </c>
+      <c r="G30" s="21">
+        <f>SUM(G21:G29)</f>
+        <v>231370.15</v>
+      </c>
+      <c r="I30" s="21">
+        <f>SUM(I21:I29)</f>
+        <v>2946395.51</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="21" t="e">
-        <f>=SUM(C25:C27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="21" t="e">
-        <f>=SUM(E25:E27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" s="21" t="e">
-        <f>=SUM(G25:G27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="21" t="e">
-        <f>=SUM(I25:I27)</f>
-        <v>#VALUE!</v>
+      <c r="C31" s="21">
+        <f>SUM(C25:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="21">
+        <f>SUM(E25:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="21">
+        <f>SUM(G25:G27)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="21">
+        <f>SUM(I25:I27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="21" t="e">
-        <f>=SUM(C30:C30)-SUM(C31:C31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E32" s="21" t="e">
-        <f>=SUM(E30:E30)-SUM(E31:E31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G32" s="21" t="e">
-        <f>=SUM(G30:G30)-SUM(G31:G31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I32" s="21" t="e">
-        <f>=SUM(I30:I30)-SUM(I31:I31)</f>
-        <v>#VALUE!</v>
+      <c r="C32" s="21">
+        <f>SUM(C30:C30)-SUM(C31:C31)</f>
+        <v>2000272.3699999999</v>
+      </c>
+      <c r="E32" s="21">
+        <f>SUM(E30:E30)-SUM(E31:E31)</f>
+        <v>1106303.8900000001</v>
+      </c>
+      <c r="G32" s="21">
+        <f>SUM(G30:G30)-SUM(G31:G31)</f>
+        <v>231370.15</v>
+      </c>
+      <c r="I32" s="21">
+        <f>SUM(I30:I30)-SUM(I31:I31)</f>
+        <v>2946395.51</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="21" t="e">
-        <f>=SUM(C19:C19)-SUM(C32:C32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" s="21" t="e">
-        <f>=SUM(E19:E19)-SUM(E32:E32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" s="21" t="e">
-        <f>=SUM(G19:G19)-SUM(G32:G32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I34" s="21" t="e">
-        <f>=SUM(I19:I19)-SUM(I32:I32)</f>
-        <v>#VALUE!</v>
+      <c r="C34" s="21">
+        <f>SUM(C19:C19)-SUM(C32:C32)</f>
+        <v>-1769271.18</v>
+      </c>
+      <c r="E34" s="21">
+        <f>SUM(E19:E19)-SUM(E32:E32)</f>
+        <v>-842109.49000000022</v>
+      </c>
+      <c r="G34" s="21">
+        <f>SUM(G19:G19)-SUM(G32:G32)</f>
+        <v>-158624.95</v>
+      </c>
+      <c r="I34" s="21">
+        <f>SUM(I19:I19)-SUM(I32:I32)</f>
+        <v>-2656758.92</v>
       </c>
     </row>
     <row r="35">
@@ -1464,15 +1467,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5318363734654" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5318363734654" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.5318363734654" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1598,51 +1598,51 @@
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="33" t="e">
-        <f>=SUM(C4:C14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E16" s="33" t="e">
-        <f>=SUM(E4:E14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" s="33" t="e">
-        <f>=SUM(G4:G14)</f>
-        <v>#VALUE!</v>
+      <c r="C16" s="33">
+        <f>SUM(C4:C14)</f>
+        <v>2651.31</v>
+      </c>
+      <c r="E16" s="33">
+        <f>SUM(E4:E14)</f>
+        <v>3803.19</v>
+      </c>
+      <c r="G16" s="33">
+        <f>SUM(G4:G14)</f>
+        <v>3276.9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="33" t="e">
-        <f>=SUM(C8:C11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E17" s="33" t="e">
-        <f>=SUM(E8:E11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" s="33" t="e">
-        <f>=SUM(G8:G11)</f>
-        <v>#VALUE!</v>
+      <c r="C17" s="33">
+        <f>SUM(C8:C11)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="33">
+        <f>SUM(E8:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="33">
+        <f>SUM(G8:G11)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="33" t="e">
-        <f>=SUM(C16:C16)-SUM(C17:C17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E19" s="33" t="e">
-        <f>=SUM(E16:E16)-SUM(E17:E17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" s="33" t="e">
-        <f>=SUM(G16:G16)-SUM(G17:G17)</f>
-        <v>#VALUE!</v>
+      <c r="C19" s="33">
+        <f>SUM(C16:C16)-SUM(C17:C17)</f>
+        <v>2651.31</v>
+      </c>
+      <c r="E19" s="33">
+        <f>SUM(E16:E16)-SUM(E17:E17)</f>
+        <v>3803.19</v>
+      </c>
+      <c r="G19" s="33">
+        <f>SUM(G16:G16)-SUM(G17:G17)</f>
+        <v>3276.9</v>
       </c>
     </row>
     <row r="21">
@@ -1694,68 +1694,68 @@
       <c r="A30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="33" t="e">
-        <f>=SUM(C21:C29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E30" s="33" t="e">
-        <f>=SUM(E21:E29)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" s="33" t="e">
-        <f>=SUM(G21:G29)</f>
-        <v>#VALUE!</v>
+      <c r="C30" s="33">
+        <f>SUM(C21:C29)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="33">
+        <f>SUM(E21:E29)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="33">
+        <f>SUM(G21:G29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="33" t="e">
-        <f>=SUM(C25:C27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="33" t="e">
-        <f>=SUM(E25:E27)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" s="33" t="e">
-        <f>=SUM(G25:G27)</f>
-        <v>#VALUE!</v>
+      <c r="C31" s="33">
+        <f>SUM(C25:C27)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="33">
+        <f>SUM(E25:E27)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="33">
+        <f>SUM(G25:G27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="33" t="e">
-        <f>=SUM(C30:C30)-SUM(C31:C31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E32" s="33" t="e">
-        <f>=SUM(E30:E30)-SUM(E31:E31)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G32" s="33" t="e">
-        <f>=SUM(G30:G30)-SUM(G31:G31)</f>
-        <v>#VALUE!</v>
+      <c r="C32" s="33">
+        <f>SUM(C30:C30)-SUM(C31:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="33">
+        <f>SUM(E30:E30)-SUM(E31:E31)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="33">
+        <f>SUM(G30:G30)-SUM(G31:G31)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="33" t="e">
-        <f>=SUM(C19:C19)-SUM(C32:C32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" s="33" t="e">
-        <f>=SUM(E19:E19)-SUM(E32:E32)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" s="33" t="e">
-        <f>=SUM(G19:G19)-SUM(G32:G32)</f>
-        <v>#VALUE!</v>
+      <c r="C34" s="33">
+        <f>SUM(C19:C19)-SUM(C32:C32)</f>
+        <v>2651.31</v>
+      </c>
+      <c r="E34" s="33">
+        <f>SUM(E19:E19)-SUM(E32:E32)</f>
+        <v>3803.19</v>
+      </c>
+      <c r="G34" s="33">
+        <f>SUM(G19:G19)-SUM(G32:G32)</f>
+        <v>3276.9</v>
       </c>
     </row>
     <row r="35">
@@ -1817,19 +1817,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="11.5318363734654" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1837,259 +1833,427 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="B4" s="0">
+        <v>55365</v>
+      </c>
+      <c r="C4" s="39">
+        <v>1014947.05</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="0">
+        <v>19766.7</v>
+      </c>
+      <c r="C5" s="39">
+        <v>362394.22</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="0">
+        <v>0</v>
+      </c>
+      <c r="C6" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B9" s="0">
+        <v>14539.5</v>
+      </c>
+      <c r="C9" s="39">
+        <v>246195.85</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
         <v>17</v>
       </c>
+      <c r="B10" s="0">
+        <v>0</v>
+      </c>
+      <c r="C10" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="B11" s="0">
+        <v>0</v>
+      </c>
+      <c r="C11" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="38">
-        <v>529.2</v>
+        <v>4112.1</v>
       </c>
       <c r="C12" s="39">
-        <v>9731.4</v>
+        <v>74636.97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="B13" s="0">
+        <v>0</v>
+      </c>
+      <c r="C13" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="B14" s="0">
+        <v>0</v>
+      </c>
+      <c r="C14" s="39">
+        <v>10750</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="39"/>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="39" t="e">
-        <f>=SUM(C4:C14)</f>
-        <v>#VALUE!</v>
+      <c r="B16" s="0">
+        <v>0</v>
+      </c>
+      <c r="C16" s="39">
+        <v>1708924.09</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="39" t="e">
-        <f>=SUM(C8:C11)</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B17" s="0">
+        <v>0</v>
+      </c>
+      <c r="C17" s="39">
+        <v>246195.85</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" s="39"/>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="39" t="e">
-        <f>=SUM(C16:C16)-SUM(C17:C17)</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B19" s="0">
+        <v>0</v>
+      </c>
+      <c r="C19" s="39">
+        <v>1462728.24</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" s="39"/>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
         <v>25</v>
       </c>
+      <c r="B21" s="0">
+        <v>0</v>
+      </c>
+      <c r="C21" s="39">
+        <v>9804898.87</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="B22" s="0">
+        <v>0</v>
+      </c>
+      <c r="C22" s="39">
+        <v>135108.7</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="B23" s="0">
+        <v>0</v>
+      </c>
+      <c r="C23" s="39">
+        <v>461951.32</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
         <v>28</v>
       </c>
+      <c r="B24" s="0">
+        <v>0</v>
+      </c>
+      <c r="C24" s="39">
+        <v>13199.34</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="B25" s="0">
+        <v>0</v>
+      </c>
+      <c r="C25" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="B26" s="0">
+        <v>0</v>
+      </c>
+      <c r="C26" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="B27" s="0">
+        <v>0</v>
+      </c>
+      <c r="C27" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
         <v>32</v>
       </c>
+      <c r="B28" s="0">
+        <v>0</v>
+      </c>
+      <c r="C28" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="B29" s="0">
+        <v>0</v>
+      </c>
+      <c r="C29" s="39">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="39" t="e">
-        <f>=SUM(C21:C29)</f>
-        <v>#VALUE!</v>
+      <c r="B30" s="0">
+        <v>0</v>
+      </c>
+      <c r="C30" s="39">
+        <v>10415158.23</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="39" t="e">
-        <f>=SUM(C25:C27)</f>
-        <v>#VALUE!</v>
+      <c r="B31" s="0">
+        <v>0</v>
+      </c>
+      <c r="C31" s="39">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="39" t="e">
-        <f>=SUM(C30:C30)-SUM(C31:C31)</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="B32" s="0">
+        <v>0</v>
+      </c>
+      <c r="C32" s="39">
+        <v>10415158.23</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" s="39"/>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="39" t="e">
-        <f>=SUM(C19:C19)-SUM(C32:C32)</f>
-        <v>#VALUE!</v>
+      <c r="C34" s="39">
+        <f>SUM(C19:C19)-SUM(C32:C32)</f>
+        <v>-8952429.99</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
         <v>38</v>
       </c>
+      <c r="B35" s="0">
+        <v>0</v>
+      </c>
+      <c r="C35" s="39">
+        <v>18969.02</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="B36" s="0">
+        <v>0</v>
+      </c>
+      <c r="C36" s="39">
+        <v>85431.03</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="B37" s="0">
+        <v>0</v>
+      </c>
+      <c r="C37" s="39">
+        <v>111143.76</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="B38" s="0">
+        <v>0</v>
+      </c>
+      <c r="C38" s="39">
+        <v>192932.25</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
         <v>42</v>
       </c>
+      <c r="B39" s="0">
+        <v>0</v>
+      </c>
+      <c r="C39" s="39">
+        <v>57559.8</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
         <v>43</v>
       </c>
+      <c r="B40" s="0">
+        <v>0</v>
+      </c>
+      <c r="C40" s="39">
+        <v>408600</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="B41" s="0">
+        <v>0</v>
+      </c>
+      <c r="C41" s="39">
+        <v>58003.2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="B42" s="0">
+        <v>0</v>
+      </c>
+      <c r="C42" s="39">
+        <v>4916100.13</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
         <v>46</v>
+      </c>
+      <c r="B43" s="0">
+        <v>0</v>
+      </c>
+      <c r="C43" s="39">
+        <v>37602.29</v>
       </c>
     </row>
   </sheetData>
@@ -2097,8 +2261,6 @@
     <mergeCell ref="A1"/>
     <mergeCell ref="A2"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <headerFooter/>
 </worksheet>

</xml_diff>